<commit_message>
Added description to readme file
</commit_message>
<xml_diff>
--- a/Output_Result.xlsx
+++ b/Output_Result.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD3"/>
@@ -714,6 +714,60 @@
         <v>3</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>20234211/24/23 -02:42:21</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ApplicationFrameHost.exe</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>35.21875</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.2163152463620963</v>
+      </c>
+      <c r="F11" t="n">
+        <v>281</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>20234211/24/23 -02:42:58</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ApplicationFrameHost.exe</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>35.21875</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.2163152463620963</v>
+      </c>
+      <c r="F12" t="n">
+        <v>558</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>